<commit_message>
Changing scripts and dataa
</commit_message>
<xml_diff>
--- a/МВ.xlsx
+++ b/МВ.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\madiyar.tolkybek\Desktop\dummy\pyda\forData\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\pyda\forData\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8856" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23016" windowHeight="8856" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
     <sheet name="Лист4" sheetId="4" r:id="rId4"/>
+    <sheet name="Лист5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="33">
   <si>
     <t>(100 + 17)</t>
   </si>
@@ -94,6 +95,39 @@
   <si>
     <t xml:space="preserve"> 17.03.20 23:00</t>
   </si>
+  <si>
+    <t>byte</t>
+  </si>
+  <si>
+    <t>type</t>
+  </si>
+  <si>
+    <t>from</t>
+  </si>
+  <si>
+    <t>to</t>
+  </si>
+  <si>
+    <t>sbyte</t>
+  </si>
+  <si>
+    <t>short</t>
+  </si>
+  <si>
+    <t>ushort</t>
+  </si>
+  <si>
+    <t>int</t>
+  </si>
+  <si>
+    <t>uint</t>
+  </si>
+  <si>
+    <t>long</t>
+  </si>
+  <si>
+    <t>ulong</t>
+  </si>
 </sst>
 </file>
 
@@ -129,7 +163,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="3"/>
@@ -161,6 +195,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -218,6 +253,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -577,6 +613,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -2559,7 +2596,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B3:I33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E34" sqref="E34"/>
     </sheetView>
   </sheetViews>
@@ -2948,8 +2985,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:I100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+    <sheetView topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="C83" sqref="C83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3748,7 +3785,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="C3:F100"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="H92" sqref="H92"/>
     </sheetView>
   </sheetViews>
@@ -4589,4 +4626,174 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B3:F11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="25.109375" customWidth="1"/>
+    <col min="5" max="5" width="39.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>255</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5">
+        <v>-128</v>
+      </c>
+      <c r="E5">
+        <v>127</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6">
+        <v>-32768</v>
+      </c>
+      <c r="E6">
+        <v>32767</v>
+      </c>
+      <c r="F6">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>65535</v>
+      </c>
+      <c r="F7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8">
+        <v>-2147483648</v>
+      </c>
+      <c r="E8">
+        <v>2147483647</v>
+      </c>
+      <c r="F8">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9">
+        <v>4294967295</v>
+      </c>
+      <c r="F9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="13">
+        <v>-9.2233720368547697E+18</v>
+      </c>
+      <c r="E10" s="13">
+        <v>9.2233720368547697E+18</v>
+      </c>
+      <c r="F10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>32</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>1.84467440737095E+19</v>
+      </c>
+      <c r="F11">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>